<commit_message>
Add template string e mapeamento de colunas
</commit_message>
<xml_diff>
--- a/teste_meu_numero.xlsx
+++ b/teste_meu_numero.xlsx
@@ -14,15 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Nome do comprador</t>
+    <t>nome</t>
   </si>
   <si>
-    <t>Número de telefone</t>
+    <t>telefone</t>
   </si>
   <si>
     <t>Victor Campos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">João </t>
+  </si>
+  <si>
+    <t>Victor Emanuel</t>
+  </si>
+  <si>
+    <t>Maria Luiza</t>
   </si>
 </sst>
 </file>
@@ -430,16 +439,28 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>5598992020511</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>5531995268389</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5">
+        <v>553181181291</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4"/>
@@ -501,11 +522,11 @@
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
     </row>

</xml_diff>